<commit_message>
Get-mdworkflow pipes to get-mdtask now
</commit_message>
<xml_diff>
--- a/Pipeline Workbook.xlsx
+++ b/Pipeline Workbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\forked\gomorpheus\morpheus-powershell\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\morpheusdata\GitHub\morpheus-powershell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF4ADF7-C690-4AA1-A7A6-BF310B1FB371}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB568B48-D957-4D9B-BA13-6E2895294EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14145" xr2:uid="{F0C7C5BD-0E1B-4666-9AB2-AE6067A3617C}"/>
+    <workbookView xWindow="-23136" yWindow="2664" windowWidth="23232" windowHeight="13152" xr2:uid="{F0C7C5BD-0E1B-4666-9AB2-AE6067A3617C}"/>
   </bookViews>
   <sheets>
     <sheet name="Morpheus.Get" sheetId="1" r:id="rId1"/>
@@ -413,6 +413,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -430,24 +448,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -769,25 +769,25 @@
   <dimension ref="A1:AO40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1328125" customWidth="1"/>
-    <col min="2" max="34" width="3.59765625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="34" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
       <c r="J1" s="31"/>
@@ -801,14 +801,14 @@
       <c r="R1" s="31"/>
       <c r="S1" s="31"/>
     </row>
-    <row r="2" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
+    <row r="2" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
       <c r="H2" s="31"/>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
@@ -822,7 +822,7 @@
       <c r="R2" s="31"/>
       <c r="S2" s="31"/>
     </row>
-    <row r="3" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="3" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -843,84 +843,84 @@
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
     </row>
-    <row r="4" spans="1:41" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:41" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="27" t="s">
+      <c r="O4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="27"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="30"/>
-      <c r="AF4" s="30"/>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="25"/>
-      <c r="AI4" s="25"/>
-      <c r="AJ4" s="25"/>
-      <c r="AK4" s="25"/>
-      <c r="AL4" s="25"/>
-      <c r="AM4" s="25"/>
-      <c r="AN4" s="25"/>
-      <c r="AO4" s="25"/>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.45">
+      <c r="R4" s="21"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="24"/>
+      <c r="AH4" s="19"/>
+      <c r="AI4" s="19"/>
+      <c r="AJ4" s="19"/>
+      <c r="AK4" s="19"/>
+      <c r="AL4" s="19"/>
+      <c r="AM4" s="19"/>
+      <c r="AN4" s="19"/>
+      <c r="AO4" s="19"/>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
@@ -943,7 +943,7 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
@@ -966,7 +966,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
@@ -989,7 +989,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
@@ -1012,7 +1012,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
@@ -1035,7 +1035,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1058,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
@@ -1081,7 +1081,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>9</v>
       </c>
@@ -1104,7 +1104,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>10</v>
       </c>
@@ -1127,7 +1127,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>11</v>
       </c>
@@ -1150,7 +1150,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>12</v>
       </c>
@@ -1173,7 +1173,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>13</v>
       </c>
@@ -1196,7 +1196,7 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>14</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>15</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>16</v>
       </c>
@@ -1261,11 +1261,11 @@
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
       <c r="P19" s="2"/>
-      <c r="Q19" s="1"/>
+      <c r="Q19" s="8"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>17</v>
       </c>
@@ -1288,7 +1288,7 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="9"/>
       <c r="C21" s="1"/>
@@ -1309,7 +1309,7 @@
       <c r="R21" s="2"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="9"/>
       <c r="C22" s="1"/>
@@ -1330,7 +1330,7 @@
       <c r="R22" s="1"/>
       <c r="S22" s="2"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="9"/>
       <c r="C23" s="1"/>
@@ -1351,7 +1351,7 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="9"/>
       <c r="C24" s="1"/>
@@ -1372,7 +1372,7 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="9"/>
       <c r="C25" s="1"/>
@@ -1393,7 +1393,7 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
       <c r="B26" s="9"/>
       <c r="C26" s="1"/>
@@ -1414,7 +1414,7 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="9"/>
       <c r="C27" s="1"/>
@@ -1435,7 +1435,7 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="9"/>
       <c r="C28" s="1"/>
@@ -1456,7 +1456,7 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="9"/>
       <c r="C29" s="1"/>
@@ -1477,7 +1477,7 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="16"/>
       <c r="B30" s="9"/>
       <c r="C30" s="1"/>
@@ -1498,7 +1498,7 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="9"/>
       <c r="C31" s="1"/>
@@ -1519,7 +1519,7 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="9"/>
       <c r="C32" s="1"/>
@@ -1540,7 +1540,7 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="9"/>
       <c r="C33" s="1"/>
@@ -1561,7 +1561,7 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="9"/>
       <c r="C34" s="1"/>
@@ -1582,7 +1582,7 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="9"/>
       <c r="C35" s="1"/>
@@ -1603,7 +1603,7 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="9"/>
       <c r="C36" s="1"/>
@@ -1624,7 +1624,7 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="9"/>
       <c r="C37" s="1"/>
@@ -1645,7 +1645,7 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="9"/>
       <c r="C38" s="1"/>
@@ -1666,7 +1666,7 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="9"/>
       <c r="C39" s="1"/>
@@ -1687,7 +1687,7 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="1:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17"/>
       <c r="B40" s="9"/>
       <c r="C40" s="1"/>

</xml_diff>

<commit_message>
get-mdpowershedule and get-mdsecuritygroups working
</commit_message>
<xml_diff>
--- a/Pipeline Workbook.xlsx
+++ b/Pipeline Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\morpheusdata\GitHub\morpheus-powershell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB568B48-D957-4D9B-BA13-6E2895294EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF3A778-8232-4E94-99B0-E9B9661FF324}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="2664" windowWidth="23232" windowHeight="13152" xr2:uid="{F0C7C5BD-0E1B-4666-9AB2-AE6067A3617C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>CMDLET</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>Get-MDWorkflow</t>
+  </si>
+  <si>
+    <t>Get-MDPowerSchedules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t>Get-MDPowerSchedule</t>
   </si>
 </sst>
 </file>
@@ -768,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F7C0EE-7D91-449C-9460-585AB588ADB1}">
   <dimension ref="A1:AO40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +904,9 @@
       <c r="Q4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="21"/>
+      <c r="R4" s="21" t="s">
+        <v>18</v>
+      </c>
       <c r="S4" s="23"/>
       <c r="T4" s="24"/>
       <c r="U4" s="24"/>
@@ -932,7 +943,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
-      <c r="J5" s="4"/>
+      <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
@@ -940,7 +951,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
-      <c r="R5" s="4"/>
+      <c r="R5" s="12"/>
       <c r="S5" s="4"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
@@ -955,7 +966,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="1"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
@@ -963,7 +974,7 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
-      <c r="R6" s="1"/>
+      <c r="R6" s="12"/>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
@@ -978,7 +989,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
@@ -986,7 +997,7 @@
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
-      <c r="R7" s="1"/>
+      <c r="R7" s="12"/>
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
@@ -1001,7 +1012,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="1"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="3"/>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
@@ -1009,7 +1020,7 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
-      <c r="R8" s="1"/>
+      <c r="R8" s="12"/>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
@@ -1024,7 +1035,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="12"/>
       <c r="K9" s="10"/>
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
@@ -1032,7 +1043,7 @@
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
-      <c r="R9" s="1"/>
+      <c r="R9" s="12"/>
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
@@ -1047,7 +1058,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="1"/>
+      <c r="J10" s="12"/>
       <c r="K10" s="10"/>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
@@ -1055,7 +1066,7 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
-      <c r="R10" s="1"/>
+      <c r="R10" s="12"/>
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
@@ -1070,7 +1081,7 @@
       <c r="G11" s="10"/>
       <c r="H11" s="2"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="12"/>
       <c r="K11" s="10"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
@@ -1078,7 +1089,7 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
-      <c r="R11" s="1"/>
+      <c r="R11" s="12"/>
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
@@ -1093,7 +1104,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="12"/>
       <c r="K12" s="10"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
@@ -1101,30 +1112,30 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
-      <c r="R12" s="1"/>
+      <c r="R12" s="12"/>
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
@@ -1139,15 +1150,17 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="10"/>
       <c r="K14" s="2"/>
       <c r="L14" s="12"/>
       <c r="M14" s="8"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="1"/>
+      <c r="Q14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14" s="12"/>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
@@ -1162,7 +1175,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="8"/>
       <c r="L15" s="2"/>
       <c r="M15" s="12"/>
@@ -1170,7 +1183,7 @@
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
-      <c r="R15" s="1"/>
+      <c r="R15" s="12"/>
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
@@ -1185,7 +1198,7 @@
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
-      <c r="J16" s="1"/>
+      <c r="J16" s="18"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="2"/>
@@ -1193,7 +1206,7 @@
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
-      <c r="R16" s="1"/>
+      <c r="R16" s="12"/>
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -1208,7 +1221,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
-      <c r="J17" s="1"/>
+      <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
@@ -1216,7 +1229,7 @@
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
-      <c r="R17" s="1"/>
+      <c r="R17" s="12"/>
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1231,7 +1244,7 @@
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
-      <c r="J18" s="1"/>
+      <c r="J18" s="18"/>
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
@@ -1239,7 +1252,7 @@
       <c r="O18" s="2"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
-      <c r="R18" s="1"/>
+      <c r="R18" s="12"/>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -1254,7 +1267,7 @@
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
-      <c r="J19" s="1"/>
+      <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
@@ -1262,7 +1275,7 @@
       <c r="O19" s="18"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="8"/>
-      <c r="R19" s="1"/>
+      <c r="R19" s="12"/>
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1277,7 +1290,7 @@
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
-      <c r="J20" s="1"/>
+      <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
@@ -1285,27 +1298,29 @@
       <c r="O20" s="18"/>
       <c r="P20" s="18"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="1"/>
+      <c r="R20" s="12"/>
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
+      <c r="A21" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
       <c r="R21" s="2"/>
       <c r="S21" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added get-mdlayout pipe from get-mdinstancetype works
</commit_message>
<xml_diff>
--- a/Pipeline Workbook.xlsx
+++ b/Pipeline Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\morpheusdata\GitHub\morpheus-powershell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9522F1-42BA-47AD-9D55-51AF42B896F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894303BA-7A8F-4520-9FF4-5D4390446372}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="2664" windowWidth="23232" windowHeight="13152" xr2:uid="{F0C7C5BD-0E1B-4666-9AB2-AE6067A3617C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>CMDLET</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Get-MDInstanceType</t>
+  </si>
+  <si>
+    <t>Get-MDLayout</t>
   </si>
 </sst>
 </file>
@@ -166,27 +169,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -305,73 +293,31 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="45"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -379,23 +325,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -412,16 +350,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F7C0EE-7D91-449C-9460-585AB588ADB1}">
   <dimension ref="A1:AO40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,48 +697,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
     </row>
     <row r="2" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
     </row>
     <row r="3" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
@@ -819,115 +762,117 @@
       <c r="S3" s="3"/>
     </row>
     <row r="4" spans="1:41" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="R4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="S4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="U4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="6"/>
-      <c r="AG4" s="6"/>
-      <c r="AH4" s="5"/>
-      <c r="AI4" s="5"/>
-      <c r="AJ4" s="5"/>
-      <c r="AK4" s="5"/>
-      <c r="AL4" s="5"/>
-      <c r="AM4" s="5"/>
-      <c r="AN4" s="5"/>
-      <c r="AO4" s="5"/>
+      <c r="V4" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="23"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="4"/>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="1"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
@@ -945,30 +890,30 @@
       <c r="AK5" s="1"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="1"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
@@ -986,30 +931,30 @@
       <c r="AK6" s="1"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="1"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
@@ -1027,30 +972,30 @@
       <c r="AK7" s="1"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="1"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
@@ -1068,30 +1013,30 @@
       <c r="AK8" s="1"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="1"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
@@ -1109,30 +1054,30 @@
       <c r="AK9" s="1"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="1"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
@@ -1150,30 +1095,30 @@
       <c r="AK10" s="1"/>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="1"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
@@ -1191,30 +1136,30 @@
       <c r="AK11" s="1"/>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="1"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
@@ -1232,30 +1177,30 @@
       <c r="AK12" s="1"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="1"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
@@ -1273,32 +1218,32 @@
       <c r="AK13" s="1"/>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="1"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
@@ -1316,30 +1261,30 @@
       <c r="AK14" s="1"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="1"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
@@ -1357,30 +1302,30 @@
       <c r="AK15" s="1"/>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="1"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
@@ -1398,30 +1343,30 @@
       <c r="AK16" s="1"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="1"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
@@ -1439,30 +1384,30 @@
       <c r="AK17" s="1"/>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="1"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
@@ -1480,30 +1425,30 @@
       <c r="AK18" s="1"/>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="1"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
@@ -1521,30 +1466,30 @@
       <c r="AK19" s="1"/>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="23"/>
-      <c r="V20" s="1"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
@@ -1562,30 +1507,30 @@
       <c r="AK20" s="1"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="23"/>
-      <c r="V21" s="1"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
@@ -1603,30 +1548,30 @@
       <c r="AK21" s="1"/>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23"/>
-      <c r="S22" s="25"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="23"/>
-      <c r="V22" s="1"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
@@ -1644,30 +1589,30 @@
       <c r="AK22" s="1"/>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="25"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="1"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
@@ -1685,30 +1630,30 @@
       <c r="AK23" s="1"/>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="25"/>
-      <c r="V24" s="1"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="10"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
@@ -1726,28 +1671,30 @@
       <c r="AK24" s="1"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
+      <c r="A25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="12"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
@@ -1765,7 +1712,7 @@
       <c r="AK25" s="1"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1804,7 +1751,7 @@
       <c r="AK26" s="1"/>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1843,7 +1790,7 @@
       <c r="AK27" s="1"/>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1882,7 +1829,7 @@
       <c r="AK28" s="1"/>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1921,7 +1868,7 @@
       <c r="AK29" s="1"/>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1960,7 +1907,7 @@
       <c r="AK30" s="1"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1999,7 +1946,7 @@
       <c r="AK31" s="1"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2038,7 +1985,7 @@
       <c r="AK32" s="1"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2077,7 +2024,7 @@
       <c r="AK33" s="1"/>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2116,7 +2063,7 @@
       <c r="AK34" s="1"/>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2155,7 +2102,7 @@
       <c r="AK35" s="1"/>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2194,7 +2141,7 @@
       <c r="AK36" s="1"/>
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2233,7 +2180,7 @@
       <c r="AK37" s="1"/>
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2272,7 +2219,7 @@
       <c r="AK38" s="1"/>
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2311,7 +2258,7 @@
       <c r="AK39" s="1"/>
     </row>
     <row r="40" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>

</xml_diff>

<commit_message>
updating logig for name and id input
</commit_message>
<xml_diff>
--- a/Pipeline Workbook.xlsx
+++ b/Pipeline Workbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\morpheusdata\GitHub\morpheus-powershell\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\forked\gomorpheus\morpheus-powershell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894303BA-7A8F-4520-9FF4-5D4390446372}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDE0298-1FA7-42DF-B535-C86419FBB967}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="2664" windowWidth="23232" windowHeight="13152" xr2:uid="{F0C7C5BD-0E1B-4666-9AB2-AE6067A3617C}"/>
+    <workbookView xWindow="68" yWindow="1185" windowWidth="14384" windowHeight="11017" xr2:uid="{F0C7C5BD-0E1B-4666-9AB2-AE6067A3617C}"/>
   </bookViews>
   <sheets>
     <sheet name="Morpheus.Get" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +165,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -332,6 +338,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -353,17 +371,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="255"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,61 +695,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F7C0EE-7D91-449C-9460-585AB588ADB1}">
   <dimension ref="A1:AO40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="34" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.1328125" customWidth="1"/>
+    <col min="2" max="34" width="3.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-    </row>
-    <row r="2" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-    </row>
-    <row r="3" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+    </row>
+    <row r="2" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+    </row>
+    <row r="3" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -761,94 +770,94 @@
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
     </row>
-    <row r="4" spans="1:41" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:41" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="P4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="21" t="s">
+      <c r="S4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="T4" s="22" t="s">
+      <c r="T4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="U4" s="22" t="s">
+      <c r="U4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="V4" s="22" t="s">
+      <c r="V4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="23"/>
-      <c r="AI4" s="23"/>
-      <c r="AJ4" s="23"/>
-      <c r="AK4" s="23"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="15"/>
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="16"/>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="16"/>
       <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
       <c r="AN4" s="4"/>
       <c r="AO4" s="4"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -889,7 +898,7 @@
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -930,7 +939,7 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -971,7 +980,7 @@
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1012,8 +1021,8 @@
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.45">
+      <c r="A9" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="10"/>
@@ -1053,8 +1062,8 @@
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.45">
+      <c r="A10" s="24" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="10"/>
@@ -1094,8 +1103,8 @@
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.45">
+      <c r="A11" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="10"/>
@@ -1135,7 +1144,7 @@
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
@@ -1176,7 +1185,7 @@
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
@@ -1217,7 +1226,7 @@
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1260,7 +1269,7 @@
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
@@ -1301,7 +1310,7 @@
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1342,7 +1351,7 @@
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1383,7 +1392,7 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1424,7 +1433,7 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1465,7 +1474,7 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1506,7 +1515,7 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
@@ -1547,7 +1556,7 @@
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
@@ -1588,7 +1597,7 @@
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
@@ -1629,7 +1638,7 @@
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
@@ -1670,7 +1679,7 @@
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
@@ -1711,7 +1720,7 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A26" s="7"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1750,7 +1759,7 @@
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A27" s="7"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1789,7 +1798,7 @@
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A28" s="7"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1828,7 +1837,7 @@
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A29" s="7"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1867,7 +1876,7 @@
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A30" s="7"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1906,7 +1915,7 @@
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A31" s="7"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1945,7 +1954,7 @@
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A32" s="7"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1984,7 +1993,7 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A33" s="7"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2023,7 +2032,7 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A34" s="7"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2062,7 +2071,7 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A35" s="7"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2101,7 +2110,7 @@
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A36" s="7"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2140,7 +2149,7 @@
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A37" s="7"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2179,7 +2188,7 @@
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A38" s="7"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2218,7 +2227,7 @@
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A39" s="7"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2257,7 +2266,7 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:37" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A40" s="8"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>

</xml_diff>

<commit_message>
Get all get by ID upto this point
</commit_message>
<xml_diff>
--- a/Pipeline Workbook.xlsx
+++ b/Pipeline Workbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\forked\gomorpheus\morpheus-powershell\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\morpheusdata\GitHub\morpheus-powershell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDE0298-1FA7-42DF-B535-C86419FBB967}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251EE385-9E38-4457-89D9-935983BC98C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68" yWindow="1185" windowWidth="14384" windowHeight="11017" xr2:uid="{F0C7C5BD-0E1B-4666-9AB2-AE6067A3617C}"/>
+    <workbookView xWindow="-23136" yWindow="2664" windowWidth="23232" windowHeight="13152" xr2:uid="{F0C7C5BD-0E1B-4666-9AB2-AE6067A3617C}"/>
   </bookViews>
   <sheets>
     <sheet name="Morpheus.Get" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,14 +168,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -188,57 +182,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -312,9 +255,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -322,56 +265,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -696,60 +627,60 @@
   <dimension ref="A1:AO40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1328125" customWidth="1"/>
-    <col min="2" max="34" width="3.59765625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="34" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="19"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-    </row>
-    <row r="2" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-    </row>
-    <row r="3" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+    </row>
+    <row r="2" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+    </row>
+    <row r="3" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -770,7 +701,7 @@
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
     </row>
-    <row r="4" spans="1:41" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:41" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
@@ -857,7 +788,7 @@
       <c r="AN4" s="4"/>
       <c r="AO4" s="4"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -898,8 +829,8 @@
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="11"/>
@@ -939,7 +870,7 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -980,8 +911,8 @@
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="10"/>
@@ -1021,8 +952,8 @@
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A9" s="24" t="s">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="10"/>
@@ -1062,8 +993,8 @@
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A10" s="24" t="s">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="10"/>
@@ -1103,8 +1034,8 @@
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="10"/>
@@ -1144,8 +1075,8 @@
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="10"/>
@@ -1185,7 +1116,7 @@
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
@@ -1226,7 +1157,7 @@
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1269,8 +1200,8 @@
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="10"/>
@@ -1310,7 +1241,7 @@
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1351,7 +1282,7 @@
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1392,7 +1323,7 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1433,7 +1364,7 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1474,8 +1405,8 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="10"/>
@@ -1515,8 +1446,8 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="10"/>
@@ -1556,8 +1487,8 @@
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="10"/>
@@ -1597,7 +1528,7 @@
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
@@ -1638,7 +1569,7 @@
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
@@ -1679,8 +1610,8 @@
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="10"/>
@@ -1720,7 +1651,7 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1759,7 +1690,7 @@
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1798,7 +1729,7 @@
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1837,7 +1768,7 @@
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1876,7 +1807,7 @@
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1915,7 +1846,7 @@
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1954,7 +1885,7 @@
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1993,7 +1924,7 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2032,7 +1963,7 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2071,7 +2002,7 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2110,7 +2041,7 @@
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2149,7 +2080,7 @@
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2188,7 +2119,7 @@
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2227,7 +2158,7 @@
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2266,7 +2197,7 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" spans="1:37" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2306,9 +2237,8 @@
       <c r="AK40" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:S2"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>